<commit_message>
Selenium Framework - Part 29
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData1.xlsx
+++ b/src/test/resources/excel/testData1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="0" windowWidth="18405" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="31275" yWindow="0" windowWidth="18405" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
   <si>
     <t>testname</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>amazonTest</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>menutext</t>
+  </si>
+  <si>
+    <t>Laptops</t>
   </si>
 </sst>
 </file>
@@ -418,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +467,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -479,6 +491,23 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -488,10 +517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +531,7 @@
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,8 +550,11 @@
       <c r="F1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -541,8 +573,11 @@
       <c r="F2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -561,8 +596,11 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -581,8 +619,11 @@
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -600,6 +641,32 @@
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>